<commit_message>
sorted category, year and code
</commit_message>
<xml_diff>
--- a/project_drivereader/data/categorized.xlsx
+++ b/project_drivereader/data/categorized.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DQAC" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TLEC" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="RESEARCH" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TLEC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="DQAC" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="exempted" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,92 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Conference Attended</t>
+          <t>Faculty achievements</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Conference Keynote</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Course plan</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Conference Presentation</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Conference Publication</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Conference Session Chair</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>fdp</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>2021-2022</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Conference Presentation</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -592,7 +516,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2021-2022</t>
+          <t>2022-2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -611,77 +535,72 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mou s</t>
+          <t>Journal Publication-Non Indexed</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
+          <t>Mou s</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Patent Filed</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Seminar Organized</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>2020-2021</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Mou s</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>2022-2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>2021-2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Book Chapter</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Journal Publication-Indexed</t>
-        </is>
-      </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Journal Publication-Non Indexed</t>
+          <t>Journal Publication-Indexed</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -691,23 +610,28 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Patent Filed</t>
+          <t>Seminar Organized</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2020-2021</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Seminar Organized</t>
+          <t>Mou s</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -716,9 +640,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A6"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -730,7 +654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,7 +663,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -767,16 +691,92 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Faculty achievements</t>
+          <t>Conference Attended</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Conference Keynote</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Course plan</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Conference Presentation</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Conference Publication</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Conference Session Chair</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>fdp</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>2021-2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Conference Presentation</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
improved format of headers
</commit_message>
<xml_diff>
--- a/project_drivereader/data/categorized.xlsx
+++ b/project_drivereader/data/categorized.xlsx
@@ -801,12 +801,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>File Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Folder name</t>
         </is>

</xml_diff>